<commit_message>
adding some more stuff
</commit_message>
<xml_diff>
--- a/testData/Write_testData.xlsx
+++ b/testData/Write_testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation Workspace\IFocus\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Automation Workspace\IFocus\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C115F1-BC8F-476A-8285-BC8C753376BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712CF6DA-309B-4CE3-B8DC-D22055D18E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="write" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>Fname</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>Ph#</t>
+  </si>
+  <si>
+    <t>First Kranthi</t>
+  </si>
+  <si>
+    <t>Last Kumar</t>
+  </si>
+  <si>
+    <t>Ph#89</t>
+  </si>
+  <si>
+    <t>Address123</t>
   </si>
 </sst>
 </file>
@@ -373,7 +385,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -381,7 +393,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.33203125" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -398,7 +411,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -412,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -426,7 +439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -438,6 +451,20 @@
       </c>
       <c r="D4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>